<commit_message>
Enhance timetable generation logic to include camp name in filenames and improve handling of Day 6 activities. Update activity descriptions for clarity and add evening and morning merge blocks for specific days. Remove outdated teacher timetable files.
</commit_message>
<xml_diff>
--- a/flute-campA-time-table.xlsx
+++ b/flute-campA-time-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmski\Desktop\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB416A28-8686-4525-8BCD-C3088381092E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033202A3-4953-4F91-91C4-821680318897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="4" xr2:uid="{4F305ACA-9255-4D6C-9A65-1407DE2CF383}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="5" xr2:uid="{4F305ACA-9255-4D6C-9A65-1407DE2CF383}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -41,12 +41,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="55">
   <si>
     <t xml:space="preserve">Time </t>
-  </si>
-  <si>
-    <t>Welcome Speech</t>
   </si>
   <si>
     <t>F1</t>
@@ -162,24 +159,6 @@
     <t>Concert call time</t>
   </si>
   <si>
-    <t>F2  Private Lesson with Stephane &amp; pianist</t>
-  </si>
-  <si>
-    <t>F6 Private Lesson with Stephane &amp; pianist</t>
-  </si>
-  <si>
-    <t>F1 Private Lesson with Stephane &amp; pianist</t>
-  </si>
-  <si>
-    <t>F3 Private Lesson with Stephane &amp; pianist</t>
-  </si>
-  <si>
-    <t>F4 Private Lesson with Stephane &amp; pianist</t>
-  </si>
-  <si>
-    <t>F5 Private Lesson with Stephane &amp; pianist</t>
-  </si>
-  <si>
     <t>Group 2, 5, 8, 9 Acting Class
 (Room Acting Class)</t>
   </si>
@@ -214,6 +193,40 @@
   <si>
     <t>Group 1, 3, 4, 6, 7 Group Activity
 (Room Group Activity)</t>
+  </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>F2  Private Lesson with Stephane RETY &amp; pianist</t>
+  </si>
+  <si>
+    <t>F6 Private Lesson with Stephane RETY &amp; pianist</t>
+  </si>
+  <si>
+    <t>F1 Private Lesson with Stephane RETY &amp; pianist</t>
+  </si>
+  <si>
+    <t>F3 Private Lesson with Stephane RETY &amp; pianist</t>
+  </si>
+  <si>
+    <t>F4 Private Lesson with Stephane RETY &amp; pianist</t>
+  </si>
+  <si>
+    <t>F5 Private Lesson with Stephane RETY &amp; pianist</t>
+  </si>
+  <si>
+    <t>Rehearsal for Faculty Concert</t>
+  </si>
+  <si>
+    <t>Lina Summer Camp of Music Faculty Concert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After concert refreshment </t>
+  </si>
+  <si>
+    <t>After Concert Dinner 
+(Pheasant-Jasmine Room, Mandarin Oriental)</t>
   </si>
 </sst>
 </file>
@@ -297,7 +310,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -582,11 +595,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -607,19 +657,87 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -629,78 +747,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -727,11 +783,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -757,48 +849,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -851,6 +901,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1189,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58029A68-0D30-435A-A4C3-6E59A3275874}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1201,13 +1266,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -1221,69 +1286,69 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
+      <c r="B3" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="41"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="D7" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="24" t="s">
+      <c r="G7" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -1323,23 +1388,23 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>3</v>
+      <c r="G11" s="14" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -1349,7 +1414,7 @@
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="24"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
     </row>
@@ -1360,7 +1425,7 @@
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="24"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
     </row>
@@ -1371,7 +1436,7 @@
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="32"/>
+      <c r="E14" s="16"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
@@ -1379,69 +1444,69 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
+      <c r="B15" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="29" t="s">
+      <c r="B19" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="10" t="s">
+      <c r="C19" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="14" t="s">
         <v>2</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
@@ -1481,22 +1546,22 @@
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="19" t="s">
+      <c r="D23" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="10"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
@@ -1504,9 +1569,9 @@
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
@@ -1515,9 +1580,9 @@
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
@@ -1526,38 +1591,38 @@
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
+      <c r="B27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="20"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="28"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
@@ -1566,9 +1631,9 @@
         <v>0.6875</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="20"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="28"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
@@ -1577,9 +1642,9 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="21"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
     </row>
@@ -1594,11 +1659,11 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>9</v>
+      <c r="B32" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
@@ -1650,16 +1715,14 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
     <mergeCell ref="E23:E26"/>
     <mergeCell ref="F23:F26"/>
     <mergeCell ref="G23:G26"/>
@@ -1676,14 +1739,16 @@
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="D23:D26"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B7:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1694,7 +1759,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D30"/>
+      <selection activeCell="C19" sqref="C19:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1705,13 +1770,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -1723,69 +1788,69 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
+      <c r="B3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="41"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="24" t="s">
+      <c r="B7" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="C7" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="E7" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="15" t="s">
         <v>6</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -1793,7 +1858,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="42"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -1804,7 +1869,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="42"/>
+      <c r="C9" s="43"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -1815,7 +1880,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="43"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -1825,23 +1890,23 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="B11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="14" t="s">
         <v>3</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -1849,7 +1914,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="42"/>
+      <c r="C12" s="43"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -1860,7 +1925,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="42"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -1871,7 +1936,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="42"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1881,69 +1946,69 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="46"/>
+      <c r="B15" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="48"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="48"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="24" t="s">
+      <c r="B19" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" s="24" t="s">
+      <c r="F19" s="15" t="s">
         <v>4</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
@@ -1951,7 +2016,7 @@
         <v>0.59375</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="42"/>
+      <c r="C20" s="43"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -1962,7 +2027,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="42"/>
+      <c r="C21" s="43"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -1973,7 +2038,7 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="12"/>
-      <c r="C22" s="43"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -1983,32 +2048,32 @@
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="19" t="s">
+      <c r="D23" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="10"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
       <c r="B24" s="11"/>
-      <c r="C24" s="42"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="11"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
@@ -2016,10 +2081,10 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B25" s="11"/>
-      <c r="C25" s="42"/>
+      <c r="C25" s="43"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
@@ -2027,39 +2092,39 @@
         <v>0.65625</v>
       </c>
       <c r="B26" s="12"/>
-      <c r="C26" s="43"/>
+      <c r="C26" s="44"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
+      <c r="B27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="16"/>
+      <c r="C28" s="40"/>
       <c r="D28" s="11"/>
-      <c r="E28" s="20"/>
+      <c r="E28" s="28"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
@@ -2068,9 +2133,9 @@
         <v>0.6875</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="16"/>
+      <c r="C29" s="40"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="20"/>
+      <c r="E29" s="28"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
@@ -2079,9 +2144,9 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="17"/>
+      <c r="C30" s="41"/>
       <c r="D30" s="12"/>
-      <c r="E30" s="21"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
     </row>
@@ -2100,11 +2165,11 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>9</v>
+      <c r="B32" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>8</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2116,7 +2181,7 @@
         <v>0.72916666666666496</v>
       </c>
       <c r="B33" s="11"/>
-      <c r="C33" s="42"/>
+      <c r="C33" s="43"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -2127,7 +2192,7 @@
         <v>0.73958333333333104</v>
       </c>
       <c r="B34" s="11"/>
-      <c r="C34" s="42"/>
+      <c r="C34" s="43"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2138,7 +2203,7 @@
         <v>0.749999999999997</v>
       </c>
       <c r="B35" s="11"/>
-      <c r="C35" s="42"/>
+      <c r="C35" s="43"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2149,7 +2214,7 @@
         <v>0.76041666666666297</v>
       </c>
       <c r="B36" s="11"/>
-      <c r="C36" s="42"/>
+      <c r="C36" s="43"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2160,7 +2225,7 @@
         <v>0.77083333333332904</v>
       </c>
       <c r="B37" s="11"/>
-      <c r="C37" s="42"/>
+      <c r="C37" s="43"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2171,7 +2236,7 @@
         <v>0.781249999999996</v>
       </c>
       <c r="B38" s="12"/>
-      <c r="C38" s="43"/>
+      <c r="C38" s="44"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2184,26 +2249,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="B15:G18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G19:G22"/>
     <mergeCell ref="B32:B38"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="F23:F26"/>
@@ -2218,6 +2263,26 @@
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="D23:D26"/>
     <mergeCell ref="E23:E26"/>
+    <mergeCell ref="B15:G18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2239,13 +2304,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -2257,77 +2322,77 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
+      <c r="B3" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="64"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="62"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="18" t="s">
+      <c r="D7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>2</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="71"/>
-      <c r="C8" s="22"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -2337,8 +2402,8 @@
       <c r="A9" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="71"/>
-      <c r="C9" s="22"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -2348,8 +2413,8 @@
       <c r="A10" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="73"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -2359,31 +2424,31 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>7</v>
+      <c r="G11" s="13" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="71"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -2393,8 +2458,8 @@
       <c r="A13" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="22"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -2404,8 +2469,8 @@
       <c r="A14" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="73"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="59"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -2415,77 +2480,77 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="66"/>
+      <c r="B15" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="64"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="48"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="48"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="69"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="67"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="70" t="s">
+      <c r="B19" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="D19" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="18" t="s">
+      <c r="F19" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="13" t="s">
         <v>6</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="71"/>
-      <c r="C20" s="22"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -2495,8 +2560,8 @@
       <c r="A21" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="22"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -2506,8 +2571,8 @@
       <c r="A22" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="72"/>
-      <c r="C22" s="73"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="59"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -2517,83 +2582,83 @@
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" s="18"/>
+      <c r="D23" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="55"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="55"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="59"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="B27" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="20"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="28"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
@@ -2601,10 +2666,10 @@
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="20"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="28"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
@@ -2612,10 +2677,10 @@
       <c r="A30" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="21"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
     </row>
@@ -2634,11 +2699,11 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>9</v>
+      <c r="B32" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>8</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2649,8 +2714,8 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="74"/>
-      <c r="C33" s="74"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -2660,8 +2725,8 @@
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="74"/>
-      <c r="C34" s="74"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2671,8 +2736,8 @@
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="74"/>
-      <c r="C35" s="74"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2682,8 +2747,8 @@
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="74"/>
-      <c r="C36" s="74"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="54"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2693,8 +2758,8 @@
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="74"/>
-      <c r="C37" s="74"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2704,8 +2769,8 @@
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="75"/>
-      <c r="C38" s="75"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2718,15 +2783,17 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
     <mergeCell ref="B3:G6"/>
     <mergeCell ref="G7:G10"/>
     <mergeCell ref="G11:G14"/>
@@ -2741,17 +2808,15 @@
     <mergeCell ref="C7:C10"/>
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="E7:E10"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="F23:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2762,7 +2827,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D30"/>
+      <selection activeCell="C23" sqref="C23:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2773,13 +2838,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -2793,69 +2858,69 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
+      <c r="B3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="41"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="30" t="s">
+      <c r="B7" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="36" t="s">
         <v>5</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -2863,7 +2928,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="16"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -2874,7 +2939,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="16"/>
+      <c r="C9" s="40"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -2885,7 +2950,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="17"/>
+      <c r="C10" s="41"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -2895,23 +2960,23 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="18" t="s">
+      <c r="B11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="18" t="s">
+      <c r="E11" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="13" t="s">
         <v>6</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -2919,7 +2984,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="16"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -2930,7 +2995,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="16"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -2941,7 +3006,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="16"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -2951,69 +3016,69 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="46"/>
+      <c r="B15" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="48"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="48"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="18" t="s">
+      <c r="B19" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="18" t="s">
+      <c r="G19" s="13" t="s">
         <v>4</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
@@ -3021,7 +3086,7 @@
         <v>0.59375</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="16"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -3032,7 +3097,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="16"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -3043,7 +3108,7 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="12"/>
-      <c r="C22" s="17"/>
+      <c r="C22" s="41"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -3053,22 +3118,22 @@
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="19" t="s">
+      <c r="D23" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="18"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
@@ -3077,8 +3142,8 @@
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
@@ -3088,8 +3153,8 @@
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
@@ -3099,37 +3164,37 @@
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="B27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="20"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="28"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
@@ -3138,9 +3203,9 @@
         <v>0.6875</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="20"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="28"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
@@ -3149,9 +3214,9 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="21"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
     </row>
@@ -3170,11 +3235,11 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>9</v>
+      <c r="B32" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>8</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -3254,19 +3319,11 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
     <mergeCell ref="G23:G26"/>
     <mergeCell ref="E27:E30"/>
     <mergeCell ref="B15:G18"/>
@@ -3283,11 +3340,19 @@
     <mergeCell ref="F23:F26"/>
     <mergeCell ref="F27:F30"/>
     <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3297,7 +3362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DEF69-E5FD-41F0-9622-94C4199D6A7C}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -3309,13 +3374,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -3330,7 +3395,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B3" s="82" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="83"/>
       <c r="D3" s="83"/>
@@ -3372,7 +3437,7 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="B7" s="76" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C7" s="88"/>
       <c r="D7" s="88"/>
@@ -3453,50 +3518,50 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="48"/>
+      <c r="B15" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="50"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="48"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="50"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="48"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="50"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="48"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="50"/>
     </row>
     <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
       <c r="B19" s="76" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C19" s="77"/>
       <c r="D19" s="77"/>
@@ -3537,20 +3602,20 @@
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>49</v>
+      <c r="D23" s="36" t="s">
+        <v>42</v>
       </c>
       <c r="E23" s="91" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="91" t="s">
         <v>29</v>
-      </c>
-      <c r="F23" s="91" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -3559,9 +3624,9 @@
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
@@ -3569,9 +3634,9 @@
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
@@ -3579,36 +3644,36 @@
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" s="18"/>
+      <c r="B27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="13"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="20"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="28"/>
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -3616,9 +3681,9 @@
         <v>0.6875</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="20"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="28"/>
       <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -3626,9 +3691,9 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="21"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="12"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -3645,11 +3710,11 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>9</v>
+      <c r="B32" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>8</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -3659,7 +3724,7 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="74"/>
+      <c r="B33" s="54"/>
       <c r="C33" s="11"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -3669,7 +3734,7 @@
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="74"/>
+      <c r="B34" s="54"/>
       <c r="C34" s="11"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -3679,7 +3744,7 @@
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="74"/>
+      <c r="B35" s="54"/>
       <c r="C35" s="11"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -3689,7 +3754,7 @@
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="74"/>
+      <c r="B36" s="54"/>
       <c r="C36" s="11"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -3699,7 +3764,7 @@
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="74"/>
+      <c r="B37" s="54"/>
       <c r="C37" s="11"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -3709,7 +3774,7 @@
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="75"/>
+      <c r="B38" s="55"/>
       <c r="C38" s="12"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -3747,8 +3812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F258A27A-E0BD-410A-AC93-E998D70178A7}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3761,17 +3826,16 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>0.41666666666666669</v>
       </c>
       <c r="B2" s="92" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>0.42708333333333331</v>
       </c>
@@ -3794,10 +3858,10 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="B6" s="93" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.46875</v>
       </c>
@@ -3843,49 +3907,49 @@
       <c r="A14" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B14" s="92" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B14" s="94" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B15" s="92"/>
+      <c r="B15" s="95"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B16" s="92"/>
+      <c r="B16" s="95"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B17" s="92"/>
+      <c r="B17" s="95"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="B18" s="96"/>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B19" s="93" t="s">
-        <v>21</v>
+      <c r="B19" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B20" s="93"/>
+      <c r="B20" s="93" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
@@ -3915,15 +3979,15 @@
       <c r="A25" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B25" s="93" t="s">
-        <v>22</v>
-      </c>
+      <c r="B25" s="93"/>
     </row>
     <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B26" s="93"/>
+      <c r="B26" s="93" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
@@ -3935,159 +3999,197 @@
       <c r="A28" s="4">
         <v>0.6875</v>
       </c>
+      <c r="B28" s="93"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>0.69791666666666696</v>
       </c>
+      <c r="B29" s="97" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>0.70833333333333304</v>
       </c>
+      <c r="B30" s="97"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
         <v>0.718749999999999</v>
       </c>
+      <c r="B31" s="97"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="4">
         <v>0.72916666666666496</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B32" s="92" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="4">
         <v>0.73958333333333104</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B33" s="92"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
         <v>0.749999999999997</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B34" s="92"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="4">
         <v>0.76041666666666297</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B35" s="92"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="4">
         <v>0.77083333333332904</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B36" s="98" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="4">
         <v>0.781249999999996</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B37" s="98"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
         <v>0.79166666666666197</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B38" s="98"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="4">
         <v>0.80208333333332804</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B39" s="98"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="4">
         <v>0.812499999999994</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B40" s="98"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="4">
         <v>0.82291666666665997</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B41" s="92" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" s="4">
         <v>0.83333333333332604</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B42" s="92"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" s="4">
         <v>0.84374999999999201</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B43" s="92"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" s="4">
         <v>0.85416666666665797</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B44" s="97" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="4">
         <v>0.86458333333332404</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B45" s="97"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" s="4">
         <v>0.87499999999999001</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B46" s="97"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" s="4">
         <v>0.88541666666665597</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B47" s="97"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" s="4">
         <v>0.89583333333332205</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B48" s="97"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" s="4">
         <v>0.90624999999998801</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B49" s="97"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" s="4">
         <v>0.91666666666665497</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B50" s="97"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" s="4">
         <v>0.92708333333332105</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52" s="4">
         <v>0.93749999999998701</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53" s="4">
         <v>0.94791666666665297</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54" s="4">
         <v>0.95833333333331905</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" s="4">
         <v>0.96874999999998501</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56" s="4">
         <v>0.97916666666665098</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57" s="4">
         <v>0.98958333333331705</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B44:B50"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>